<commit_message>
skill-effect 1차 완 / skill table 시작 (category 데이터를 skill info에서 skill 로 이동)
</commit_message>
<xml_diff>
--- a/로스트아크/데이터테이블/Skill_Info_Table.xlsx
+++ b/로스트아크/데이터테이블/Skill_Info_Table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sky20\Desktop\진선\GameDesign\로스트아크\데이터테이블\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF46C5E1-28D9-4001-94DD-A8DE802DE515}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AD92CFA-96D7-4088-B604-2DE50D5A2CA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{8E3DD992-F5CA-43CA-A90A-D3D2390C4793}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8E3DD992-F5CA-43CA-A90A-D3D2390C4793}"/>
   </bookViews>
   <sheets>
     <sheet name="Schema" sheetId="2" r:id="rId1"/>
@@ -301,273 +301,6 @@
         </r>
       </text>
     </comment>
-    <comment ref="F8" authorId="0" shapeId="0" xr:uid="{2B369155-C557-42B7-BF94-4F1DF83919E5}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="맑은 고딕"/>
-            <family val="3"/>
-            <charset val="129"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[스킬 종류]</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="맑은 고딕"/>
-            <family val="3"/>
-            <charset val="129"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="맑은 고딕"/>
-            <family val="3"/>
-            <charset val="129"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve">BASIC_ATTACK </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="맑은 고딕"/>
-            <family val="3"/>
-            <charset val="129"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>: 기본 공격(평타)</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="맑은 고딕"/>
-            <family val="3"/>
-            <charset val="129"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve">
-MOVEMENT </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="맑은 고딕"/>
-            <family val="3"/>
-            <charset val="129"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>: 이동기</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="맑은 고딕"/>
-            <family val="3"/>
-            <charset val="129"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve">
-STAND_UP</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="맑은 고딕"/>
-            <family val="3"/>
-            <charset val="129"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve"> : 기상기</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="맑은 고딕"/>
-            <family val="3"/>
-            <charset val="129"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve">
-IDENTITY</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="맑은 고딕"/>
-            <family val="3"/>
-            <charset val="129"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve"> : 아이덴티티 스킬</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="맑은 고딕"/>
-            <family val="3"/>
-            <charset val="129"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve">
-AWAKENING</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="맑은 고딕"/>
-            <family val="3"/>
-            <charset val="129"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve"> : 각성기
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="맑은 고딕"/>
-            <family val="3"/>
-            <charset val="129"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>HYPER_AWAKENING</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="맑은 고딕"/>
-            <family val="3"/>
-            <charset val="129"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve"> : 초각성기</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="맑은 고딕"/>
-            <family val="3"/>
-            <charset val="129"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve">
-NORMAL_0 </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="맑은 고딕"/>
-            <family val="3"/>
-            <charset val="129"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>: 일반 스킬</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="맑은 고딕"/>
-            <family val="3"/>
-            <charset val="129"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve">
-NORMAL_1 </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="맑은 고딕"/>
-            <family val="3"/>
-            <charset val="129"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>: 일반 스킬 상세 분류 1 (ex: 소울이터 - 살귀 스킬)</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="맑은 고딕"/>
-            <family val="3"/>
-            <charset val="129"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve">
-NORMAL_2 </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="맑은 고딕"/>
-            <family val="3"/>
-            <charset val="129"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>: 일반 스킬 상세 분류 2 (ex: 소울이터 - 망자 스킬)</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="맑은 고딕"/>
-            <family val="3"/>
-            <charset val="129"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve">
-NORMAL_3 </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="맑은 고딕"/>
-            <family val="3"/>
-            <charset val="129"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>: 일반 스킬 상세 분류 3 (ex: 소울이터 - 사신 스킬)</t>
-        </r>
-      </text>
-    </comment>
   </commentList>
 </comments>
 </file>
@@ -965,7 +698,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="61">
   <si>
     <t>설명</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1152,181 +885,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">스킬을 사용하는 </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>클래스 id</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> (Class_Table.xlsx의 id)</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>스킬 정보 ID의 넘버링 규칙</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">'고유의 특징'에 따라 분류되는 </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">스킬 종류 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(메모 참고)</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>창술사 ID</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>5번 스킬</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>05</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>305</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>→</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>313</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>10</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>브레이커 ID</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>10번 스킬</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">[예시 1] </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>id = 30505</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">[예시 2] </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>id = 31310</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">OOO/OO -&gt; </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">클래스 id </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">/ </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>스킬 No.</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
       <rPr>
         <b/>
         <sz val="10"/>
@@ -1352,10 +910,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>enum</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>AWAKENING</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1364,12 +918,80 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>ex) 창술사의 일반 스킬 분류 : 난무(FLURRY) &amp; 집중(FOCUS)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <t>NORMAL_2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IDENTITY</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BASIC_ATTACK</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NORMAL_3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>마우스 지점에 공격을 가한다. 도약하여 전방을 바라보며 후방으로 4m 가량 공중으로 점프한다. 이후 창에 기를 집중하고 선택한 지점에 창을 던진다. 창이 지점에 떨어지며 {dmg_1}의 피해를 주고 서서히 폭발하여 {dmg_2}, {dmg_2}, {dmg_3}, {dmg_3}, {dmg_4}의 피해를 주고 마지막 {dmg_4}의 피해를 주며 날려버린다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>정신을 집중 한 뒤 순간적으로 전방에 창을 찔러 {dmg_1}의 피해를 주며 창을 당겨 {dmg_1}의 피해를 주며 적들을 당겨온다. 이후 창을 휘둘러 {dmg_2}의 피해를 {hit_cnt_2}회 주고 찌르는 공격으로 {dmg_3}의 피해를 {hit_cnt_3}회 준다. 피니쉬로 전방으로 8m가량 전진하며 이동 공격을 하여 적에게 {dmg_4}의 피해를 주며 날려버린다. 이동 중 모험가 및 몬스터와 충돌이 무시된다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>lm_skill_01_26.png</t>
+  </si>
+  <si>
+    <t>lm_skill_01_27.png</t>
+  </si>
+  <si>
+    <t>lm_skill_01_18.png</t>
+  </si>
+  <si>
+    <t>lm_skill_01_25.png</t>
+  </si>
+  <si>
+    <t>lm_skill_01_23.png</t>
+  </si>
+  <si>
+    <t>lm_skill_01_15.png</t>
+  </si>
+  <si>
+    <t>ifm_skill_01_23.png</t>
+  </si>
+  <si>
+    <t>ifm_skill_01_22.png</t>
+  </si>
+  <si>
+    <t>ifm_skill_01_26.png</t>
+  </si>
+  <si>
+    <t>ifm_skill_01_27.png</t>
+  </si>
+  <si>
+    <t>ifm_skill_01_25.png</t>
+  </si>
+  <si>
+    <t>ifm_skill_01_28.png</t>
+  </si>
+  <si>
+    <t>se_skill_01_20.png</t>
+  </si>
+  <si>
+    <t>se_skill_01_21.png</t>
+  </si>
+  <si>
+    <t>se_skill_01_18.png</t>
+  </si>
+  <si>
+    <t>se_skill_01_19.png</t>
   </si>
   <si>
     <r>
-      <t xml:space="preserve">-&gt; </t>
+      <t xml:space="preserve">스킬을 사용하는 </t>
     </r>
     <r>
       <rPr>
@@ -1381,87 +1003,8 @@
         <charset val="129"/>
         <scheme val="minor"/>
       </rPr>
-      <t>클래스 별 일반 스킬 분류</t>
+      <t>클래스의 고유 id</t>
     </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>에 해당되는 값</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>category =</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> NORMAL_1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>NORMAL_2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, … </t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>NORMAL_2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>IDENTITY</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BASIC_ATTACK</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>NORMAL_3</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1474,7 +1017,7 @@
     <numFmt numFmtId="177" formatCode="0_);[Red]\(0\)"/>
     <numFmt numFmtId="178" formatCode="00"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1602,14 +1145,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color theme="1"/>
-      <name val="맑은 고딕"/>
-      <family val="3"/>
-      <charset val="129"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="8"/>
       <color indexed="81"/>
@@ -1627,7 +1162,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1672,18 +1207,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFD5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
+        <fgColor rgb="FFC00000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="38">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -1978,185 +1507,13 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2217,9 +1574,6 @@
     <xf numFmtId="178" fontId="5" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="5" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -2283,68 +1637,20 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="34" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="33" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="177" fontId="5" fillId="8" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="177" fontId="5" fillId="8" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2355,59 +1661,17 @@
     <xf numFmtId="0" fontId="9" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="35" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="36" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="37" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2430,55 +1694,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>233082</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>2244936</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>214551</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="그림 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8C942CFA-3603-6F7F-BF91-F1BF3ECE7F44}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3980329" y="4043082"/>
-          <a:ext cx="2011854" cy="1335140"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2778,9 +1993,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF385D5D-99E2-46DF-BA33-B40AE917BBB4}">
-  <dimension ref="B1:M24"/>
+  <dimension ref="B1:G21"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
@@ -2791,250 +2006,156 @@
     <col min="3" max="3" width="4.3984375" style="12" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="18.09765625" style="2" customWidth="1"/>
     <col min="6" max="6" width="56.8984375" style="2" customWidth="1"/>
-    <col min="7" max="9" width="8.69921875" style="3" customWidth="1"/>
-    <col min="10" max="11" width="8.796875" style="3"/>
-    <col min="12" max="12" width="10.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.8984375" style="3" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="8.796875" style="3"/>
+    <col min="7" max="7" width="8.69921875" style="3" customWidth="1"/>
+    <col min="8" max="16384" width="8.796875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13" ht="18" thickBot="1" x14ac:dyDescent="0.45"/>
-    <row r="2" spans="2:13" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C2" s="63" t="s">
+    <row r="1" spans="2:7" ht="18" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="2" spans="2:7" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="C2" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="64"/>
-      <c r="E2" s="65"/>
-      <c r="H2" s="66" t="s">
-        <v>36</v>
-      </c>
-      <c r="I2" s="67"/>
-      <c r="J2" s="67"/>
-      <c r="K2" s="68"/>
-    </row>
-    <row r="3" spans="2:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C3" s="26" t="s">
+      <c r="D2" s="47"/>
+      <c r="E2" s="48"/>
+    </row>
+    <row r="3" spans="2:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="C3" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="23" t="s">
+      <c r="D3" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="23" t="s">
+      <c r="E3" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="27" t="s">
+      <c r="F3" s="26" t="s">
         <v>0</v>
       </c>
       <c r="G3" s="4"/>
-      <c r="H3" s="72" t="s">
-        <v>49</v>
-      </c>
-      <c r="I3" s="73"/>
-      <c r="J3" s="73"/>
-      <c r="K3" s="74"/>
-    </row>
-    <row r="4" spans="2:13" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C4" s="24" t="s">
+    </row>
+    <row r="4" spans="2:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="C4" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="25" t="s">
+      <c r="D4" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="22" t="s">
+      <c r="E4" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="28" t="s">
+      <c r="F4" s="27" t="s">
         <v>25</v>
       </c>
       <c r="G4" s="4"/>
-      <c r="H4" s="75"/>
-      <c r="I4" s="76"/>
-      <c r="J4" s="76"/>
-      <c r="K4" s="77"/>
-    </row>
-    <row r="5" spans="2:13" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B5" s="40" t="s">
+    </row>
+    <row r="5" spans="2:7" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B5" s="39" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="29">
+      <c r="C5" s="28">
         <v>1</v>
       </c>
-      <c r="D5" s="30" t="s">
+      <c r="D5" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="31" t="s">
+      <c r="E5" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="F5" s="32" t="s">
+      <c r="F5" s="31" t="s">
         <v>29</v>
       </c>
       <c r="G5" s="4"/>
-      <c r="H5" s="78" t="s">
-        <v>47</v>
-      </c>
-      <c r="I5" s="79"/>
-      <c r="J5" s="79"/>
-      <c r="K5" s="82" t="s">
-        <v>42</v>
-      </c>
-      <c r="L5" s="46" t="s">
-        <v>41</v>
-      </c>
-      <c r="M5" s="50" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.4">
-      <c r="B6" s="41" t="s">
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.4">
+      <c r="B6" s="40" t="s">
         <v>32</v>
       </c>
-      <c r="C6" s="33">
+      <c r="C6" s="32">
         <v>2</v>
       </c>
-      <c r="D6" s="34" t="s">
+      <c r="D6" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="35" t="s">
+      <c r="E6" s="34" t="s">
         <v>28</v>
       </c>
-      <c r="F6" s="36" t="s">
+      <c r="F6" s="35" t="s">
         <v>33</v>
       </c>
       <c r="G6" s="4"/>
-      <c r="H6" s="80"/>
-      <c r="I6" s="81"/>
-      <c r="J6" s="81"/>
-      <c r="K6" s="83"/>
-      <c r="L6" s="47" t="s">
-        <v>38</v>
-      </c>
-      <c r="M6" s="48" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.4">
-      <c r="B7" s="41" t="s">
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.4">
+      <c r="B7" s="40"/>
+      <c r="C7" s="49">
+        <v>3</v>
+      </c>
+      <c r="D7" s="50" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="51" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" s="52" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B8" s="40" t="s">
         <v>32</v>
       </c>
-      <c r="C7" s="33">
-        <v>3</v>
-      </c>
-      <c r="D7" s="34" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" s="35" t="s">
+      <c r="C8" s="32">
+        <v>4</v>
+      </c>
+      <c r="D8" s="33" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="34" t="s">
         <v>28</v>
       </c>
-      <c r="F7" s="36" t="s">
+      <c r="F8" s="35" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.4">
+      <c r="B9" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="32">
+        <v>5</v>
+      </c>
+      <c r="D9" s="33" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9" s="34" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="H7" s="69"/>
-      <c r="I7" s="70"/>
-      <c r="J7" s="70"/>
-      <c r="K7" s="70"/>
-      <c r="L7" s="70"/>
-      <c r="M7" s="71"/>
-    </row>
-    <row r="8" spans="2:13" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C8" s="52">
-        <v>4</v>
-      </c>
-      <c r="D8" s="53" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="54" t="s">
-        <v>51</v>
-      </c>
-      <c r="F8" s="55" t="s">
-        <v>37</v>
-      </c>
-      <c r="H8" s="57" t="s">
-        <v>48</v>
-      </c>
-      <c r="I8" s="58"/>
-      <c r="J8" s="58"/>
-      <c r="K8" s="61" t="s">
-        <v>42</v>
-      </c>
-      <c r="L8" s="49" t="s">
-        <v>43</v>
-      </c>
-      <c r="M8" s="51" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="9" spans="2:13" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B9" s="41" t="s">
-        <v>32</v>
-      </c>
-      <c r="C9" s="33">
-        <v>5</v>
-      </c>
-      <c r="D9" s="34" t="s">
-        <v>10</v>
-      </c>
-      <c r="E9" s="35" t="s">
-        <v>28</v>
-      </c>
-      <c r="F9" s="36" t="s">
-        <v>34</v>
-      </c>
-      <c r="H9" s="59"/>
-      <c r="I9" s="60"/>
-      <c r="J9" s="60"/>
-      <c r="K9" s="62"/>
-      <c r="L9" s="42" t="s">
-        <v>45</v>
-      </c>
-      <c r="M9" s="43" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.4">
-      <c r="B10" s="41" t="s">
-        <v>32</v>
-      </c>
-      <c r="C10" s="33">
-        <v>6</v>
-      </c>
-      <c r="D10" s="34" t="s">
-        <v>30</v>
-      </c>
-      <c r="E10" s="35" t="s">
-        <v>28</v>
-      </c>
-      <c r="F10" s="36" t="s">
-        <v>50</v>
-      </c>
-      <c r="J10" s="45"/>
-      <c r="K10" s="44"/>
-    </row>
-    <row r="11" spans="2:13" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C11" s="13"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="21"/>
-      <c r="F11" s="15"/>
-    </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.4">
-      <c r="F14" s="38"/>
-    </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.4">
-      <c r="F15" s="39"/>
-    </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.4">
-      <c r="F16" s="39" t="s">
-        <v>56</v>
-      </c>
+    </row>
+    <row r="10" spans="2:7" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="C10" s="13"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="15"/>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.4">
+      <c r="F13" s="38"/>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.4">
+      <c r="F14" s="41"/>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.4">
+      <c r="F15" s="38"/>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.4">
+      <c r="F16" s="6"/>
     </row>
     <row r="17" spans="6:6" x14ac:dyDescent="0.4">
-      <c r="F17" s="56" t="s">
-        <v>55</v>
-      </c>
+      <c r="F17" s="6"/>
     </row>
     <row r="18" spans="6:6" x14ac:dyDescent="0.4">
-      <c r="F18" s="39" t="s">
-        <v>54</v>
-      </c>
+      <c r="F18" s="6"/>
     </row>
     <row r="19" spans="6:6" x14ac:dyDescent="0.4">
       <c r="F19" s="6"/>
@@ -3045,31 +2166,14 @@
     <row r="21" spans="6:6" x14ac:dyDescent="0.4">
       <c r="F21" s="6"/>
     </row>
-    <row r="22" spans="6:6" x14ac:dyDescent="0.4">
-      <c r="F22" s="6"/>
-    </row>
-    <row r="23" spans="6:6" x14ac:dyDescent="0.4">
-      <c r="F23" s="6"/>
-    </row>
-    <row r="24" spans="6:6" x14ac:dyDescent="0.4">
-      <c r="F24" s="6"/>
-    </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="H8:J9"/>
-    <mergeCell ref="K8:K9"/>
+  <mergeCells count="1">
     <mergeCell ref="C2:E2"/>
-    <mergeCell ref="H2:K2"/>
-    <mergeCell ref="H7:M7"/>
-    <mergeCell ref="H3:K4"/>
-    <mergeCell ref="H5:J6"/>
-    <mergeCell ref="K5:K6"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -3077,17 +2181,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC540C7E-1D9A-4204-BA37-262FBD0C3DDD}">
   <dimension ref="A1:AG18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="18.3984375" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="15.8984375" style="9" customWidth="1"/>
+    <col min="2" max="2" width="15.8984375" style="9" customWidth="1"/>
+    <col min="3" max="3" width="17.3984375" style="9" customWidth="1"/>
     <col min="4" max="4" width="11.19921875" style="11" customWidth="1"/>
     <col min="5" max="5" width="14.09765625" style="9" customWidth="1"/>
-    <col min="6" max="7" width="15.8984375" style="9" customWidth="1"/>
+    <col min="6" max="6" width="50.5" style="9" customWidth="1"/>
+    <col min="7" max="7" width="15.8984375" style="9" customWidth="1"/>
     <col min="8" max="8" width="15.69921875" style="7" customWidth="1"/>
     <col min="9" max="10" width="15.69921875" style="6" customWidth="1"/>
     <col min="11" max="11" width="18.69921875" style="6" customWidth="1"/>
@@ -3106,7 +2212,7 @@
       <c r="B1" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="43" t="s">
         <v>9</v>
       </c>
       <c r="D1" s="19" t="s">
@@ -3115,10 +2221,10 @@
       <c r="E1" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="18" t="s">
+      <c r="F1" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="20" t="s">
+      <c r="G1" s="45" t="s">
         <v>30</v>
       </c>
       <c r="H1" s="5"/>
@@ -3148,22 +2254,28 @@
       <c r="AF1" s="2"/>
       <c r="AG1" s="2"/>
     </row>
-    <row r="2" spans="1:33" s="3" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:33" s="3" customFormat="1" ht="93.6" x14ac:dyDescent="0.4">
       <c r="A2" s="8" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="9">
         <v>30500</v>
       </c>
-      <c r="C2" s="9"/>
+      <c r="C2" s="42" t="s">
+        <v>4</v>
+      </c>
       <c r="D2" s="10">
         <v>305</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
+        <v>36</v>
+      </c>
+      <c r="F2" s="37" t="s">
+        <v>42</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>44</v>
+      </c>
       <c r="H2" s="5"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
@@ -3191,22 +2303,28 @@
       <c r="AF2" s="2"/>
       <c r="AG2" s="2"/>
     </row>
-    <row r="3" spans="1:33" s="3" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:33" s="3" customFormat="1" ht="93.6" x14ac:dyDescent="0.4">
       <c r="A3" s="8" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="9">
         <v>30501</v>
       </c>
-      <c r="C3" s="9"/>
+      <c r="C3" s="42" t="s">
+        <v>5</v>
+      </c>
       <c r="D3" s="10">
         <v>305</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
+        <v>36</v>
+      </c>
+      <c r="F3" s="44" t="s">
+        <v>43</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>45</v>
+      </c>
       <c r="H3" s="5"/>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
@@ -3241,15 +2359,19 @@
       <c r="B4" s="9">
         <v>30502</v>
       </c>
-      <c r="C4" s="9"/>
+      <c r="C4" s="42" t="s">
+        <v>6</v>
+      </c>
       <c r="D4" s="10">
         <v>305</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
       <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
+      <c r="G4" s="9" t="s">
+        <v>46</v>
+      </c>
       <c r="H4" s="5"/>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
@@ -3284,15 +2406,19 @@
       <c r="B5" s="9">
         <v>30503</v>
       </c>
-      <c r="C5" s="9"/>
+      <c r="C5" s="42" t="s">
+        <v>7</v>
+      </c>
       <c r="D5" s="10">
         <v>305</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>57</v>
+        <v>38</v>
       </c>
       <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
+      <c r="G5" s="9" t="s">
+        <v>47</v>
+      </c>
       <c r="H5" s="5"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
@@ -3327,15 +2453,19 @@
       <c r="B6" s="9">
         <v>30504</v>
       </c>
-      <c r="C6" s="9"/>
+      <c r="C6" s="42" t="s">
+        <v>18</v>
+      </c>
       <c r="D6" s="10">
         <v>305</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>57</v>
+        <v>38</v>
       </c>
       <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
+      <c r="G6" s="9" t="s">
+        <v>48</v>
+      </c>
       <c r="H6" s="5"/>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
@@ -3370,15 +2500,19 @@
       <c r="B7" s="9">
         <v>30505</v>
       </c>
-      <c r="C7" s="9"/>
+      <c r="C7" s="42" t="s">
+        <v>19</v>
+      </c>
       <c r="D7" s="10">
         <v>305</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
       <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
+      <c r="G7" s="9" t="s">
+        <v>49</v>
+      </c>
       <c r="H7" s="5"/>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
@@ -3413,15 +2547,19 @@
       <c r="B8" s="9">
         <v>31300</v>
       </c>
-      <c r="C8" s="9"/>
+      <c r="C8" s="42" t="s">
+        <v>13</v>
+      </c>
       <c r="D8" s="10">
         <v>313</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
+      <c r="G8" s="9" t="s">
+        <v>50</v>
+      </c>
       <c r="H8" s="5"/>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
@@ -3456,15 +2594,19 @@
       <c r="B9" s="9">
         <v>31301</v>
       </c>
-      <c r="C9" s="9"/>
+      <c r="C9" s="42" t="s">
+        <v>14</v>
+      </c>
       <c r="D9" s="10">
         <v>313</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
+      <c r="G9" s="9" t="s">
+        <v>51</v>
+      </c>
       <c r="H9" s="5"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
@@ -3499,11 +2641,17 @@
       <c r="B10" s="9">
         <v>31302</v>
       </c>
+      <c r="C10" s="42" t="s">
+        <v>15</v>
+      </c>
       <c r="D10" s="10">
         <v>313</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>58</v>
+        <v>39</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:33" x14ac:dyDescent="0.4">
@@ -3513,11 +2661,17 @@
       <c r="B11" s="9">
         <v>31303</v>
       </c>
+      <c r="C11" s="42" t="s">
+        <v>17</v>
+      </c>
       <c r="D11" s="10">
         <v>313</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>59</v>
+        <v>40</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:33" x14ac:dyDescent="0.4">
@@ -3527,11 +2681,17 @@
       <c r="B12" s="9">
         <v>31304</v>
       </c>
+      <c r="C12" s="42" t="s">
+        <v>16</v>
+      </c>
       <c r="D12" s="10">
         <v>313</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>58</v>
+        <v>39</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:33" x14ac:dyDescent="0.4">
@@ -3541,11 +2701,17 @@
       <c r="B13" s="9">
         <v>40500</v>
       </c>
+      <c r="C13" s="42" t="s">
+        <v>20</v>
+      </c>
       <c r="D13" s="11">
         <v>405</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>52</v>
+        <v>36</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:33" x14ac:dyDescent="0.4">
@@ -3555,11 +2721,17 @@
       <c r="B14" s="9">
         <v>40501</v>
       </c>
+      <c r="C14" s="42" t="s">
+        <v>21</v>
+      </c>
       <c r="D14" s="11">
         <v>405</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>52</v>
+        <v>36</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:33" x14ac:dyDescent="0.4">
@@ -3569,11 +2741,17 @@
       <c r="B15" s="9">
         <v>40502</v>
       </c>
+      <c r="C15" s="42" t="s">
+        <v>23</v>
+      </c>
       <c r="D15" s="11">
         <v>405</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>60</v>
+        <v>41</v>
+      </c>
+      <c r="G15" s="9" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="16" spans="1:33" x14ac:dyDescent="0.4">
@@ -3583,15 +2761,26 @@
       <c r="B16" s="9">
         <v>40503</v>
       </c>
+      <c r="C16" s="42" t="s">
+        <v>22</v>
+      </c>
       <c r="D16" s="11">
         <v>405</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.4">
-      <c r="B18" s="37"/>
+        <v>41</v>
+      </c>
+      <c r="G16" s="9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.4">
+      <c r="G17" s="9" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.4">
+      <c r="B18" s="36"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>